<commit_message>
fixing ruby bug (#6)
* testing numerics for food game... sooo hard😓😩

* integer linear programming☺️有解辣！

* integer linear programming☺️有解辣！

* fixed ruby bug
</commit_message>
<xml_diff>
--- a/fruit_ninja_flutter/assets/data/nutritions.xlsx
+++ b/fruit_ninja_flutter/assets/data/nutritions.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yinghaiyu/Main/DesktopMain/STUDY/GameDevelopment/fruit_ninja_flutter/assets/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{746BF423-94B1-234E-817E-ABA395D53390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{DA9F3EB8-DAC5-9F4E-9D11-786439D1CA2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15860" yWindow="-21100" windowWidth="38400" windowHeight="21100"/>
+    <workbookView xWindow="-22540" yWindow="-21600" windowWidth="16620" windowHeight="21600" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="nutritions" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="95">
   <si>
     <t>watermelon</t>
   </si>
@@ -118,6 +119,12 @@
     <t>alcohol</t>
   </si>
   <si>
+    <t>lower</t>
+  </si>
+  <si>
+    <t>upper</t>
+  </si>
+  <si>
     <t>20 lower</t>
   </si>
   <si>
@@ -167,13 +174,145 @@
   </si>
   <si>
     <t>20 year to day</t>
+  </si>
+  <si>
+    <t>water(g)</t>
+  </si>
+  <si>
+    <t>energy(kcal)</t>
+  </si>
+  <si>
+    <t>protein(g)</t>
+  </si>
+  <si>
+    <t>fat(g)</t>
+  </si>
+  <si>
+    <t>carb(g)</t>
+  </si>
+  <si>
+    <t>fiber(g)</t>
+  </si>
+  <si>
+    <t>sugar(g)</t>
+  </si>
+  <si>
+    <t>calcium(mg)</t>
+  </si>
+  <si>
+    <t>iron(mg)</t>
+  </si>
+  <si>
+    <t>magnesium(mg)</t>
+  </si>
+  <si>
+    <t>phosphorus(mg)</t>
+  </si>
+  <si>
+    <t>potassium(mg)</t>
+  </si>
+  <si>
+    <t>sodium(mg)</t>
+  </si>
+  <si>
+    <t>zinc(mg)</t>
+  </si>
+  <si>
+    <t>copper(mg)</t>
+  </si>
+  <si>
+    <t>manganese(mg)</t>
+  </si>
+  <si>
+    <t>selenium(ug)</t>
+  </si>
+  <si>
+    <t>VC(mg)</t>
+  </si>
+  <si>
+    <t>VB(mg)</t>
+  </si>
+  <si>
+    <t>VA(ug)</t>
+  </si>
+  <si>
+    <t>VD(ug)</t>
+  </si>
+  <si>
+    <t>VK(ug)</t>
+  </si>
+  <si>
+    <t>caffeine(mg)</t>
+  </si>
+  <si>
+    <t>alcohol(mg)</t>
+  </si>
+  <si>
+    <t>broccoli</t>
+  </si>
+  <si>
+    <t>pink salmon</t>
+  </si>
+  <si>
+    <t>Chicken; broilers or fryers; leg; meat and skin; raw</t>
+  </si>
+  <si>
+    <t>Bread; whole-wheat; commercially prepared; toasted</t>
+  </si>
+  <si>
+    <t>arugula</t>
+  </si>
+  <si>
+    <t>Beef; ribeye cap steak; boneless; separable lean only; trimmed to 0" fat; choice; raw</t>
+  </si>
+  <si>
+    <t>egg</t>
+  </si>
+  <si>
+    <t>Corn, sweet, white, raw</t>
+  </si>
+  <si>
+    <t>Alcoholic beverage, beer, light</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alcoholic beverage, distilled, vodka, 80 proof	</t>
+  </si>
+  <si>
+    <t>Beverages, coffee, brewed, espresso, restaurant-prepared</t>
+  </si>
+  <si>
+    <t>Rice noodles, cooked</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Rice and vermicelli mix, rice pilaf flavor, unprepared</t>
+  </si>
+  <si>
+    <t>Beverages, rice milk, unsweetened</t>
+  </si>
+  <si>
+    <t>Yogurt, plain, whole milk</t>
+  </si>
+  <si>
+    <t>Tofu, dried-frozen (koyadofu)</t>
+  </si>
+  <si>
+    <t>Bread, cornbread, dry mix, enriched (includes corn muffin mix)</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>100g</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -307,6 +446,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -650,9 +795,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1010,8 +1156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P25" sqref="P25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1033,73 +1179,73 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O1" t="s">
+        <v>37</v>
+      </c>
+      <c r="P1" t="s">
         <v>42</v>
       </c>
-      <c r="H1" t="s">
+      <c r="Q1" t="s">
         <v>43</v>
       </c>
-      <c r="I1" t="s">
-        <v>47</v>
-      </c>
-      <c r="L1" t="s">
-        <v>32</v>
-      </c>
-      <c r="M1" t="s">
-        <v>33</v>
-      </c>
-      <c r="N1" t="s">
-        <v>34</v>
-      </c>
-      <c r="O1" t="s">
-        <v>35</v>
-      </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
+        <v>38</v>
+      </c>
+      <c r="S1" t="s">
+        <v>39</v>
+      </c>
+      <c r="T1" t="s">
         <v>40</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="U1" t="s">
         <v>41</v>
       </c>
-      <c r="R1" t="s">
-        <v>36</v>
-      </c>
-      <c r="S1" t="s">
-        <v>37</v>
-      </c>
-      <c r="T1" t="s">
-        <v>38</v>
-      </c>
-      <c r="U1" t="s">
-        <v>39</v>
-      </c>
       <c r="W1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="X1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="Y1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="Z1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="AA1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="AB1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="AC1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="AD1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="AE1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="AF1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.2">
@@ -1128,7 +1274,7 @@
         <v>5000</v>
       </c>
       <c r="I2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L2">
         <f>G2*W2</f>
@@ -1227,7 +1373,7 @@
         <v>2400</v>
       </c>
       <c r="I3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L3">
         <f>G3*W3</f>
@@ -1329,7 +1475,7 @@
         <v>60</v>
       </c>
       <c r="J4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="L4">
         <f>G4*W4*60</f>
@@ -1527,7 +1673,7 @@
         <v>300</v>
       </c>
       <c r="I6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L6">
         <f t="shared" ref="L6:L25" si="2">G6*W6</f>
@@ -1626,7 +1772,7 @@
         <v>70</v>
       </c>
       <c r="I7" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L7">
         <f t="shared" si="2"/>
@@ -1701,7 +1847,7 @@
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B8">
         <v>280</v>
@@ -1725,7 +1871,7 @@
         <v>36</v>
       </c>
       <c r="I8" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L8">
         <f t="shared" si="2"/>
@@ -1824,7 +1970,7 @@
         <v>2500</v>
       </c>
       <c r="I9" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L9">
         <f t="shared" si="2"/>
@@ -1923,7 +2069,7 @@
         <v>45</v>
       </c>
       <c r="I10" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L10">
         <f t="shared" si="2"/>
@@ -2022,7 +2168,7 @@
         <v>350</v>
       </c>
       <c r="I11" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L11">
         <f t="shared" si="2"/>
@@ -2121,7 +2267,7 @@
         <v>4000</v>
       </c>
       <c r="I12" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L12">
         <f t="shared" si="2"/>
@@ -2220,7 +2366,7 @@
         <v>4700</v>
       </c>
       <c r="I13" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L13">
         <f t="shared" si="2"/>
@@ -2319,7 +2465,7 @@
         <v>2300</v>
       </c>
       <c r="I14" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L14">
         <f t="shared" si="2"/>
@@ -2418,7 +2564,7 @@
         <v>40</v>
       </c>
       <c r="I15" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L15">
         <f t="shared" si="2"/>
@@ -2517,7 +2663,7 @@
         <v>10</v>
       </c>
       <c r="I16" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L16">
         <f t="shared" si="2"/>
@@ -2616,7 +2762,7 @@
         <v>11</v>
       </c>
       <c r="I17" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L17">
         <f t="shared" si="2"/>
@@ -2715,7 +2861,7 @@
         <v>400</v>
       </c>
       <c r="I18" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L18">
         <f t="shared" si="2"/>
@@ -2814,7 +2960,7 @@
         <v>2000</v>
       </c>
       <c r="I19" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L19">
         <f t="shared" si="2"/>
@@ -2913,7 +3059,7 @@
         <v>100</v>
       </c>
       <c r="I20" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L20">
         <f t="shared" si="2"/>
@@ -3012,7 +3158,7 @@
         <v>3000</v>
       </c>
       <c r="I21" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L21">
         <f t="shared" si="2"/>
@@ -3111,7 +3257,7 @@
         <v>100</v>
       </c>
       <c r="I22" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L22">
         <f t="shared" si="2"/>
@@ -3210,7 +3356,7 @@
         <v>120</v>
       </c>
       <c r="I23" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L23">
         <f t="shared" si="2"/>
@@ -3309,7 +3455,7 @@
         <v>400</v>
       </c>
       <c r="I24" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L24">
         <f t="shared" si="2"/>
@@ -3408,7 +3554,7 @@
         <v>30000</v>
       </c>
       <c r="I25" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L25">
         <f t="shared" si="2"/>
@@ -3485,4 +3631,1933 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="5.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K1" t="s">
+        <v>59</v>
+      </c>
+      <c r="L1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N1" t="s">
+        <v>62</v>
+      </c>
+      <c r="O1" t="s">
+        <v>63</v>
+      </c>
+      <c r="P1" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R1" t="s">
+        <v>66</v>
+      </c>
+      <c r="S1" t="s">
+        <v>67</v>
+      </c>
+      <c r="T1" t="s">
+        <v>68</v>
+      </c>
+      <c r="U1" t="s">
+        <v>69</v>
+      </c>
+      <c r="V1" t="s">
+        <v>70</v>
+      </c>
+      <c r="W1" t="s">
+        <v>71</v>
+      </c>
+      <c r="X1" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2">
+        <v>500</v>
+      </c>
+      <c r="D2">
+        <v>1200</v>
+      </c>
+      <c r="E2">
+        <v>0.8</v>
+      </c>
+      <c r="F2">
+        <v>0.2</v>
+      </c>
+      <c r="G2">
+        <v>130</v>
+      </c>
+      <c r="H2">
+        <v>25</v>
+      </c>
+      <c r="I2">
+        <v>2</v>
+      </c>
+      <c r="J2">
+        <v>1000</v>
+      </c>
+      <c r="K2">
+        <v>8</v>
+      </c>
+      <c r="L2">
+        <v>320</v>
+      </c>
+      <c r="M2">
+        <v>700</v>
+      </c>
+      <c r="N2">
+        <v>3500</v>
+      </c>
+      <c r="O2">
+        <v>500</v>
+      </c>
+      <c r="P2">
+        <v>8</v>
+      </c>
+      <c r="Q2">
+        <v>0.9</v>
+      </c>
+      <c r="R2">
+        <v>1.8</v>
+      </c>
+      <c r="S2">
+        <v>55</v>
+      </c>
+      <c r="T2">
+        <v>75</v>
+      </c>
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2">
+        <v>700</v>
+      </c>
+      <c r="W2">
+        <v>15</v>
+      </c>
+      <c r="X2">
+        <v>75</v>
+      </c>
+      <c r="Y2">
+        <v>1</v>
+      </c>
+      <c r="Z2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3">
+        <v>5000</v>
+      </c>
+      <c r="D3">
+        <v>2400</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>0.35</v>
+      </c>
+      <c r="G3">
+        <v>300</v>
+      </c>
+      <c r="H3">
+        <v>70</v>
+      </c>
+      <c r="I3">
+        <v>36</v>
+      </c>
+      <c r="J3">
+        <v>2500</v>
+      </c>
+      <c r="K3">
+        <v>45</v>
+      </c>
+      <c r="L3">
+        <v>350</v>
+      </c>
+      <c r="M3">
+        <v>4000</v>
+      </c>
+      <c r="N3">
+        <v>4700</v>
+      </c>
+      <c r="O3">
+        <v>2300</v>
+      </c>
+      <c r="P3">
+        <v>40</v>
+      </c>
+      <c r="Q3">
+        <v>10</v>
+      </c>
+      <c r="R3">
+        <v>11</v>
+      </c>
+      <c r="S3">
+        <v>400</v>
+      </c>
+      <c r="T3">
+        <v>2000</v>
+      </c>
+      <c r="U3">
+        <v>100</v>
+      </c>
+      <c r="V3">
+        <v>3000</v>
+      </c>
+      <c r="W3">
+        <v>100</v>
+      </c>
+      <c r="X3">
+        <v>120</v>
+      </c>
+      <c r="Y3">
+        <v>400</v>
+      </c>
+      <c r="Z3">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>4130</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1360</v>
+      </c>
+      <c r="E4">
+        <v>27.6</v>
+      </c>
+      <c r="F4">
+        <v>6.78</v>
+      </c>
+      <c r="G4">
+        <v>341</v>
+      </c>
+      <c r="H4">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="I4">
+        <v>280</v>
+      </c>
+      <c r="J4">
+        <v>316</v>
+      </c>
+      <c r="K4">
+        <v>10.8</v>
+      </c>
+      <c r="L4">
+        <v>452</v>
+      </c>
+      <c r="M4">
+        <v>497</v>
+      </c>
+      <c r="N4">
+        <v>5060</v>
+      </c>
+      <c r="O4">
+        <v>45.2</v>
+      </c>
+      <c r="P4">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="Q4">
+        <v>1.9</v>
+      </c>
+      <c r="R4">
+        <v>1.72</v>
+      </c>
+      <c r="S4">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="T4">
+        <v>366</v>
+      </c>
+      <c r="U4">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="V4">
+        <v>1270</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5">
+        <v>83.6</v>
+      </c>
+      <c r="D5">
+        <v>65</v>
+      </c>
+      <c r="E5">
+        <v>0.15</v>
+      </c>
+      <c r="F5">
+        <v>0.16</v>
+      </c>
+      <c r="G5">
+        <v>15.6</v>
+      </c>
+      <c r="H5">
+        <v>2.1</v>
+      </c>
+      <c r="I5">
+        <v>13.3</v>
+      </c>
+      <c r="J5">
+        <v>6</v>
+      </c>
+      <c r="K5">
+        <v>0.02</v>
+      </c>
+      <c r="L5">
+        <v>4.7</v>
+      </c>
+      <c r="M5">
+        <v>10</v>
+      </c>
+      <c r="N5">
+        <v>104</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <v>0.02</v>
+      </c>
+      <c r="Q5">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="R5">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>5.7</v>
+      </c>
+      <c r="U5">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="V5">
+        <v>2</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>1</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6">
+        <v>75.3</v>
+      </c>
+      <c r="D6">
+        <v>98</v>
+      </c>
+      <c r="E6">
+        <v>0.74</v>
+      </c>
+      <c r="F6">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="G6">
+        <v>23</v>
+      </c>
+      <c r="H6">
+        <v>1.7</v>
+      </c>
+      <c r="I6">
+        <v>15.8</v>
+      </c>
+      <c r="J6">
+        <v>5</v>
+      </c>
+      <c r="K6">
+        <v>0.4</v>
+      </c>
+      <c r="L6">
+        <v>28</v>
+      </c>
+      <c r="M6">
+        <v>22</v>
+      </c>
+      <c r="N6">
+        <v>326</v>
+      </c>
+      <c r="O6">
+        <v>4</v>
+      </c>
+      <c r="P6">
+        <v>0.16</v>
+      </c>
+      <c r="Q6">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="R6">
+        <v>0.25800000000000001</v>
+      </c>
+      <c r="S6">
+        <v>2.5</v>
+      </c>
+      <c r="T6">
+        <v>12.3</v>
+      </c>
+      <c r="U6">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="V6">
+        <v>1</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6">
+        <v>0.1</v>
+      </c>
+      <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7">
+        <v>73.2</v>
+      </c>
+      <c r="D7">
+        <v>160</v>
+      </c>
+      <c r="E7">
+        <v>670</v>
+      </c>
+      <c r="F7">
+        <v>14.7</v>
+      </c>
+      <c r="G7">
+        <v>8.5299999999999994</v>
+      </c>
+      <c r="H7">
+        <v>6.7</v>
+      </c>
+      <c r="I7">
+        <v>0.66</v>
+      </c>
+      <c r="J7">
+        <v>12</v>
+      </c>
+      <c r="K7">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="L7">
+        <v>29</v>
+      </c>
+      <c r="M7">
+        <v>52</v>
+      </c>
+      <c r="N7">
+        <v>485</v>
+      </c>
+      <c r="O7">
+        <v>7</v>
+      </c>
+      <c r="P7">
+        <v>0.64</v>
+      </c>
+      <c r="Q7">
+        <v>0.19</v>
+      </c>
+      <c r="R7">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="S7">
+        <v>0.4</v>
+      </c>
+      <c r="T7">
+        <v>10</v>
+      </c>
+      <c r="U7">
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="V7">
+        <v>7</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="X7">
+        <v>21</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8" s="2">
+        <v>90</v>
+      </c>
+      <c r="D8" s="2">
+        <v>39</v>
+      </c>
+      <c r="E8" s="2">
+        <v>2.57</v>
+      </c>
+      <c r="F8" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G8" s="2">
+        <v>6.27</v>
+      </c>
+      <c r="H8" s="2">
+        <v>2.4</v>
+      </c>
+      <c r="I8" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="J8" s="2">
+        <v>46</v>
+      </c>
+      <c r="K8" s="2">
+        <v>0.69</v>
+      </c>
+      <c r="L8" s="2">
+        <v>21</v>
+      </c>
+      <c r="M8" s="2">
+        <v>67</v>
+      </c>
+      <c r="N8" s="2">
+        <v>303</v>
+      </c>
+      <c r="O8" s="2">
+        <v>36</v>
+      </c>
+      <c r="P8" s="2">
+        <v>0.42</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="R8" s="2">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="S8" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="T8" s="2">
+        <v>91.3</v>
+      </c>
+      <c r="U8" s="2">
+        <v>0.191</v>
+      </c>
+      <c r="V8" s="2">
+        <v>8</v>
+      </c>
+      <c r="W8" s="2">
+        <v>0</v>
+      </c>
+      <c r="X8" s="2">
+        <v>102</v>
+      </c>
+      <c r="Y8" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="2">
+        <v>75.5</v>
+      </c>
+      <c r="D9" s="2">
+        <v>127</v>
+      </c>
+      <c r="E9" s="2">
+        <v>20.5</v>
+      </c>
+      <c r="F9" s="2">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0</v>
+      </c>
+      <c r="J9" s="2">
+        <v>7</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0.38</v>
+      </c>
+      <c r="L9" s="2">
+        <v>27</v>
+      </c>
+      <c r="M9" s="2">
+        <v>261</v>
+      </c>
+      <c r="N9" s="2">
+        <v>366</v>
+      </c>
+      <c r="O9" s="2">
+        <v>75</v>
+      </c>
+      <c r="P9" s="2">
+        <v>0.39</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>6.3E-2</v>
+      </c>
+      <c r="R9" s="2">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="S9" s="2">
+        <v>31.4</v>
+      </c>
+      <c r="T9" s="2">
+        <v>0</v>
+      </c>
+      <c r="U9" s="2">
+        <v>0.61099999999999999</v>
+      </c>
+      <c r="V9" s="2">
+        <v>35</v>
+      </c>
+      <c r="W9" s="2">
+        <v>10.9</v>
+      </c>
+      <c r="X9" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="Y9" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C10" s="2">
+        <v>67.3</v>
+      </c>
+      <c r="D10" s="2">
+        <v>214</v>
+      </c>
+      <c r="E10" s="2">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="F10" s="2">
+        <v>16</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0.17</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0</v>
+      </c>
+      <c r="J10" s="2">
+        <v>9</v>
+      </c>
+      <c r="K10" s="2">
+        <v>0.69</v>
+      </c>
+      <c r="L10" s="2">
+        <v>19</v>
+      </c>
+      <c r="M10" s="2">
+        <v>155</v>
+      </c>
+      <c r="N10" s="2">
+        <v>203</v>
+      </c>
+      <c r="O10" s="2">
+        <v>84</v>
+      </c>
+      <c r="P10" s="2">
+        <v>1.47</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="R10" s="2">
+        <v>1.6E-2</v>
+      </c>
+      <c r="S10" s="2">
+        <v>18</v>
+      </c>
+      <c r="T10" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="U10" s="2">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="V10" s="2">
+        <v>28</v>
+      </c>
+      <c r="W10" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="X10" s="2">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="Y10" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11" s="2">
+        <v>66.5</v>
+      </c>
+      <c r="D11" s="2">
+        <v>187</v>
+      </c>
+      <c r="E11" s="2">
+        <v>19.5</v>
+      </c>
+      <c r="F11" s="2">
+        <v>11.4</v>
+      </c>
+      <c r="G11" s="2">
+        <v>1.75</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0</v>
+      </c>
+      <c r="I11" s="2">
+        <v>0</v>
+      </c>
+      <c r="J11" s="2">
+        <v>6</v>
+      </c>
+      <c r="K11" s="2">
+        <v>2.64</v>
+      </c>
+      <c r="L11" s="2">
+        <v>24</v>
+      </c>
+      <c r="M11" s="2">
+        <v>210</v>
+      </c>
+      <c r="N11" s="2">
+        <v>357</v>
+      </c>
+      <c r="O11" s="2">
+        <v>88</v>
+      </c>
+      <c r="P11" s="2">
+        <v>7.8</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="R11" s="2">
+        <v>0</v>
+      </c>
+      <c r="S11" s="2">
+        <v>25.5</v>
+      </c>
+      <c r="T11" s="2">
+        <v>0</v>
+      </c>
+      <c r="U11" s="2">
+        <v>0.39</v>
+      </c>
+      <c r="V11" s="2">
+        <v>2</v>
+      </c>
+      <c r="W11" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="X11" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="Y11" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" s="2">
+        <v>91.7</v>
+      </c>
+      <c r="D12" s="2">
+        <v>25</v>
+      </c>
+      <c r="E12" s="2">
+        <v>2.58</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="G12" s="2">
+        <v>3.65</v>
+      </c>
+      <c r="H12" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="I12" s="2">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="J12" s="2">
+        <v>160</v>
+      </c>
+      <c r="K12" s="2">
+        <v>1.46</v>
+      </c>
+      <c r="L12" s="2">
+        <v>47</v>
+      </c>
+      <c r="M12" s="2">
+        <v>52</v>
+      </c>
+      <c r="N12" s="2">
+        <v>369</v>
+      </c>
+      <c r="O12" s="2">
+        <v>27</v>
+      </c>
+      <c r="P12" s="2">
+        <v>0.47</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="R12" s="2">
+        <v>0.32100000000000001</v>
+      </c>
+      <c r="S12" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="T12" s="2">
+        <v>15</v>
+      </c>
+      <c r="U12" s="2">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="V12" s="2">
+        <v>119</v>
+      </c>
+      <c r="W12" s="2">
+        <v>0</v>
+      </c>
+      <c r="X12" s="2">
+        <v>109</v>
+      </c>
+      <c r="Y12" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C13" s="2">
+        <v>24.2</v>
+      </c>
+      <c r="D13" s="2">
+        <v>306</v>
+      </c>
+      <c r="E13" s="2">
+        <v>16.3</v>
+      </c>
+      <c r="F13" s="2">
+        <v>4.07</v>
+      </c>
+      <c r="G13" s="2">
+        <v>51.2</v>
+      </c>
+      <c r="H13" s="2">
+        <v>7.5</v>
+      </c>
+      <c r="I13" s="2">
+        <v>5.77</v>
+      </c>
+      <c r="J13" s="2">
+        <v>130</v>
+      </c>
+      <c r="K13" s="2">
+        <v>2.96</v>
+      </c>
+      <c r="L13" s="2">
+        <v>99</v>
+      </c>
+      <c r="M13" s="2">
+        <v>303</v>
+      </c>
+      <c r="N13" s="2">
+        <v>326</v>
+      </c>
+      <c r="O13" s="2">
+        <v>565</v>
+      </c>
+      <c r="P13" s="2">
+        <v>2.15</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>67</v>
+      </c>
+      <c r="R13" s="2">
+        <v>2.54</v>
+      </c>
+      <c r="S13" s="2">
+        <v>52.6</v>
+      </c>
+      <c r="T13" s="2">
+        <v>0</v>
+      </c>
+      <c r="U13" s="2">
+        <v>0.23699999999999999</v>
+      </c>
+      <c r="V13" s="2">
+        <v>0</v>
+      </c>
+      <c r="W13" s="2">
+        <v>0</v>
+      </c>
+      <c r="X13" s="2">
+        <v>9</v>
+      </c>
+      <c r="Y13" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14" s="2">
+        <v>4.07</v>
+      </c>
+      <c r="D14" s="2">
+        <v>558</v>
+      </c>
+      <c r="E14" s="2">
+        <v>48.1</v>
+      </c>
+      <c r="F14" s="2">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="G14" s="2">
+        <v>1.87</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0</v>
+      </c>
+      <c r="J14" s="2">
+        <v>220</v>
+      </c>
+      <c r="K14" s="2">
+        <v>6.97</v>
+      </c>
+      <c r="L14" s="2">
+        <v>44.6</v>
+      </c>
+      <c r="M14" s="2">
+        <v>770</v>
+      </c>
+      <c r="N14" s="2">
+        <v>468</v>
+      </c>
+      <c r="O14" s="2">
+        <v>485</v>
+      </c>
+      <c r="P14" s="2">
+        <v>5.0199999999999996</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>0</v>
+      </c>
+      <c r="R14" s="2">
+        <v>0</v>
+      </c>
+      <c r="S14" s="2">
+        <v>0</v>
+      </c>
+      <c r="T14" s="2">
+        <v>0</v>
+      </c>
+      <c r="U14" s="2">
+        <v>0</v>
+      </c>
+      <c r="V14" s="2">
+        <v>0</v>
+      </c>
+      <c r="W14" s="2">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="X14" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C15" s="2">
+        <v>76</v>
+      </c>
+      <c r="D15" s="2">
+        <v>86</v>
+      </c>
+      <c r="E15" s="2">
+        <v>3.22</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1.18</v>
+      </c>
+      <c r="G15" s="2">
+        <v>19</v>
+      </c>
+      <c r="H15" s="2">
+        <v>2.7</v>
+      </c>
+      <c r="I15" s="2">
+        <v>3.22</v>
+      </c>
+      <c r="J15" s="2">
+        <v>2</v>
+      </c>
+      <c r="K15" s="2">
+        <v>0.52</v>
+      </c>
+      <c r="L15" s="2">
+        <v>37</v>
+      </c>
+      <c r="M15" s="2">
+        <v>89</v>
+      </c>
+      <c r="N15" s="2">
+        <v>270</v>
+      </c>
+      <c r="O15" s="2">
+        <v>15</v>
+      </c>
+      <c r="P15" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="R15" s="2">
+        <v>0.161</v>
+      </c>
+      <c r="S15" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="T15" s="2">
+        <v>6.8</v>
+      </c>
+      <c r="U15" s="2">
+        <v>0</v>
+      </c>
+      <c r="V15" s="2">
+        <v>0</v>
+      </c>
+      <c r="W15" s="2">
+        <v>0</v>
+      </c>
+      <c r="X15" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="Y15" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C16" s="2">
+        <v>94.9</v>
+      </c>
+      <c r="D16" s="2">
+        <v>29</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.24</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0</v>
+      </c>
+      <c r="G16" s="2">
+        <v>1.64</v>
+      </c>
+      <c r="H16" s="2">
+        <v>0</v>
+      </c>
+      <c r="I16" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="J16" s="2">
+        <v>4</v>
+      </c>
+      <c r="K16" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="L16" s="2">
+        <v>5</v>
+      </c>
+      <c r="M16" s="2">
+        <v>12</v>
+      </c>
+      <c r="N16" s="2">
+        <v>21</v>
+      </c>
+      <c r="O16" s="2">
+        <v>4</v>
+      </c>
+      <c r="P16" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="Q16" s="2">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="R16" s="2">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="S16" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="T16" s="2">
+        <v>0</v>
+      </c>
+      <c r="U16" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="V16" s="2">
+        <v>0</v>
+      </c>
+      <c r="W16" s="2">
+        <v>0</v>
+      </c>
+      <c r="X16" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="2">
+        <v>3100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C17" s="2">
+        <v>66.599999999999994</v>
+      </c>
+      <c r="D17" s="2">
+        <v>231</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0</v>
+      </c>
+      <c r="G17" s="2">
+        <v>0</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0</v>
+      </c>
+      <c r="I17" s="2">
+        <v>0</v>
+      </c>
+      <c r="J17" s="2">
+        <v>0</v>
+      </c>
+      <c r="K17" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="L17" s="2">
+        <v>0</v>
+      </c>
+      <c r="M17" s="2">
+        <v>5</v>
+      </c>
+      <c r="N17" s="2">
+        <v>1</v>
+      </c>
+      <c r="O17" s="2">
+        <v>1</v>
+      </c>
+      <c r="P17" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="R17" s="2">
+        <v>0</v>
+      </c>
+      <c r="S17" s="2">
+        <v>0</v>
+      </c>
+      <c r="T17" s="2">
+        <v>0</v>
+      </c>
+      <c r="U17" s="2">
+        <v>0</v>
+      </c>
+      <c r="V17" s="2">
+        <v>0</v>
+      </c>
+      <c r="W17" s="2">
+        <v>0</v>
+      </c>
+      <c r="X17" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="2">
+        <v>33400</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C18" s="2">
+        <v>97.8</v>
+      </c>
+      <c r="D18" s="2">
+        <v>9</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0.18</v>
+      </c>
+      <c r="G18" s="2">
+        <v>1.67</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0</v>
+      </c>
+      <c r="I18" s="2">
+        <v>0</v>
+      </c>
+      <c r="J18" s="2">
+        <v>2</v>
+      </c>
+      <c r="K18" s="2">
+        <v>0.13</v>
+      </c>
+      <c r="L18" s="2">
+        <v>80</v>
+      </c>
+      <c r="M18" s="2">
+        <v>7</v>
+      </c>
+      <c r="N18" s="2">
+        <v>115</v>
+      </c>
+      <c r="O18" s="2">
+        <v>14</v>
+      </c>
+      <c r="P18" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="R18" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="S18" s="2">
+        <v>0</v>
+      </c>
+      <c r="T18" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="U18" s="2">
+        <v>2E-3</v>
+      </c>
+      <c r="V18" s="2">
+        <v>0</v>
+      </c>
+      <c r="W18" s="2">
+        <v>0</v>
+      </c>
+      <c r="X18" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="Y18" s="2">
+        <v>212</v>
+      </c>
+      <c r="Z18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C19" s="2">
+        <v>73.8</v>
+      </c>
+      <c r="D19" s="2">
+        <v>108</v>
+      </c>
+      <c r="E19" s="2">
+        <v>1.79</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="G19" s="2">
+        <v>24</v>
+      </c>
+      <c r="H19" s="2">
+        <v>1</v>
+      </c>
+      <c r="I19" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="J19" s="2">
+        <v>4</v>
+      </c>
+      <c r="K19" s="2">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="L19" s="2">
+        <v>3</v>
+      </c>
+      <c r="M19" s="2">
+        <v>20</v>
+      </c>
+      <c r="N19" s="2">
+        <v>4</v>
+      </c>
+      <c r="O19" s="2">
+        <v>19</v>
+      </c>
+      <c r="P19" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="Q19" s="2">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="R19" s="2">
+        <v>0.114</v>
+      </c>
+      <c r="S19" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="T19" s="2">
+        <v>0</v>
+      </c>
+      <c r="U19" s="2">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="V19" s="2">
+        <v>0</v>
+      </c>
+      <c r="W19" s="2">
+        <v>0</v>
+      </c>
+      <c r="X19" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C20" s="2">
+        <v>8.0399999999999991</v>
+      </c>
+      <c r="D20" s="2">
+        <v>359</v>
+      </c>
+      <c r="E20" s="2">
+        <v>10.4</v>
+      </c>
+      <c r="F20" s="2">
+        <v>1.37</v>
+      </c>
+      <c r="G20" s="2">
+        <v>76.3</v>
+      </c>
+      <c r="H20" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="I20" s="2">
+        <v>1.53</v>
+      </c>
+      <c r="J20" s="2">
+        <v>83</v>
+      </c>
+      <c r="K20" s="2">
+        <v>2.44</v>
+      </c>
+      <c r="L20" s="2">
+        <v>32</v>
+      </c>
+      <c r="M20" s="2">
+        <v>154</v>
+      </c>
+      <c r="N20" s="2">
+        <v>188</v>
+      </c>
+      <c r="O20" s="2">
+        <v>1300</v>
+      </c>
+      <c r="P20" s="2">
+        <v>1.01</v>
+      </c>
+      <c r="Q20" s="2">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="R20" s="2">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="S20" s="2">
+        <v>32.4</v>
+      </c>
+      <c r="T20" s="2">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="U20" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="V20" s="2">
+        <v>4</v>
+      </c>
+      <c r="W20" s="2">
+        <v>0</v>
+      </c>
+      <c r="X20" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="Y20" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z20" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C21" s="2">
+        <v>89.3</v>
+      </c>
+      <c r="D21" s="2">
+        <v>47</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F21" s="2">
+        <v>0.97</v>
+      </c>
+      <c r="G21" s="2">
+        <v>9.17</v>
+      </c>
+      <c r="H21" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="I21" s="2">
+        <v>5.28</v>
+      </c>
+      <c r="J21" s="2">
+        <v>118</v>
+      </c>
+      <c r="K21" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="L21" s="2">
+        <v>11</v>
+      </c>
+      <c r="M21" s="2">
+        <v>56</v>
+      </c>
+      <c r="N21" s="2">
+        <v>27</v>
+      </c>
+      <c r="O21" s="2">
+        <v>39</v>
+      </c>
+      <c r="P21" s="2">
+        <v>0.13</v>
+      </c>
+      <c r="Q21" s="2">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="R21" s="2">
+        <v>0.28199999999999997</v>
+      </c>
+      <c r="S21" s="2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="T21" s="2">
+        <v>0</v>
+      </c>
+      <c r="U21" s="2">
+        <v>3.9E-2</v>
+      </c>
+      <c r="V21" s="2">
+        <v>63</v>
+      </c>
+      <c r="W21" s="2">
+        <v>1</v>
+      </c>
+      <c r="X21" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="Y21" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z21" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C22" s="2">
+        <v>87.9</v>
+      </c>
+      <c r="D22" s="2">
+        <v>61</v>
+      </c>
+      <c r="E22" s="2">
+        <v>3.47</v>
+      </c>
+      <c r="F22" s="2">
+        <v>3.25</v>
+      </c>
+      <c r="G22" s="2">
+        <v>4.66</v>
+      </c>
+      <c r="H22" s="2">
+        <v>0</v>
+      </c>
+      <c r="I22" s="2">
+        <v>4.66</v>
+      </c>
+      <c r="J22" s="2">
+        <v>121</v>
+      </c>
+      <c r="K22" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="L22" s="2">
+        <v>12</v>
+      </c>
+      <c r="M22" s="2">
+        <v>95</v>
+      </c>
+      <c r="N22" s="2">
+        <v>155</v>
+      </c>
+      <c r="O22" s="2">
+        <v>46</v>
+      </c>
+      <c r="P22" s="2">
+        <v>0.59</v>
+      </c>
+      <c r="Q22" s="2">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="R22" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="S22" s="2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="T22" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="U22" s="2">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="V22" s="2">
+        <v>27</v>
+      </c>
+      <c r="W22" s="2">
+        <v>2</v>
+      </c>
+      <c r="X22" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="Y22" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z22" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C23" s="2">
+        <v>5.78</v>
+      </c>
+      <c r="D23" s="2">
+        <v>477</v>
+      </c>
+      <c r="E23" s="2">
+        <v>52.5</v>
+      </c>
+      <c r="F23" s="2">
+        <v>30.3</v>
+      </c>
+      <c r="G23" s="2">
+        <v>10</v>
+      </c>
+      <c r="H23" s="2">
+        <v>7.2</v>
+      </c>
+      <c r="I23" s="2">
+        <v>0</v>
+      </c>
+      <c r="J23" s="2">
+        <v>364</v>
+      </c>
+      <c r="K23" s="2">
+        <v>9.73</v>
+      </c>
+      <c r="L23" s="2">
+        <v>59</v>
+      </c>
+      <c r="M23" s="2">
+        <v>483</v>
+      </c>
+      <c r="N23" s="2">
+        <v>20</v>
+      </c>
+      <c r="O23" s="2">
+        <v>6</v>
+      </c>
+      <c r="P23" s="2">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="Q23" s="2">
+        <v>1.18</v>
+      </c>
+      <c r="R23" s="2">
+        <v>3.69</v>
+      </c>
+      <c r="S23" s="2">
+        <v>54.3</v>
+      </c>
+      <c r="T23" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="U23" s="2">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="V23" s="2">
+        <v>26</v>
+      </c>
+      <c r="W23" s="2">
+        <v>0</v>
+      </c>
+      <c r="X23" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y23" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z23" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24" s="2">
+        <v>7.8</v>
+      </c>
+      <c r="D24" s="2">
+        <v>418</v>
+      </c>
+      <c r="E24" s="2">
+        <v>7</v>
+      </c>
+      <c r="F24" s="2">
+        <v>12.2</v>
+      </c>
+      <c r="G24" s="2">
+        <v>69.5</v>
+      </c>
+      <c r="H24" s="2">
+        <v>6.5</v>
+      </c>
+      <c r="I24" s="2">
+        <v>20.3</v>
+      </c>
+      <c r="J24" s="2">
+        <v>57</v>
+      </c>
+      <c r="K24" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="L24" s="2">
+        <v>24</v>
+      </c>
+      <c r="M24" s="2">
+        <v>489</v>
+      </c>
+      <c r="N24" s="2">
+        <v>113</v>
+      </c>
+      <c r="O24" s="2">
+        <v>817</v>
+      </c>
+      <c r="P24" s="2">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="Q24" s="2">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="R24" s="2">
+        <v>0.315</v>
+      </c>
+      <c r="S24" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="T24" s="2">
+        <v>0.128</v>
+      </c>
+      <c r="U24" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="V24" s="2">
+        <v>19</v>
+      </c>
+      <c r="W24" s="2">
+        <v>0</v>
+      </c>
+      <c r="X24" s="2">
+        <v>5</v>
+      </c>
+      <c r="Y24" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z24" s="2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>